<commit_message>
mapas de conceitos e planilha geral de perfil de indicadores
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Alergias/Modelo lógicoAlergiaIPS.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Alergias/Modelo lógicoAlergiaIPS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Entregaveis/1.RepositorioSemantico/Alergias/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Alergias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9898DE0C-C8B3-8F43-BF1D-A92324F48FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE7050D-E097-EA4D-9CF5-0D649A95747D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="1200" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3100" yWindow="1040" windowWidth="30240" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALergias" sheetId="1" r:id="rId1"/>
@@ -993,7 +993,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1274,7 +1274,7 @@
       <c r="F9" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="14" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="16" t="s">
@@ -1415,9 +1415,10 @@
     <hyperlink ref="A9" r:id="rId11" xr:uid="{7FDF6F92-C7FD-B14F-8A30-255692D0FC2D}"/>
     <hyperlink ref="G11" r:id="rId12" xr:uid="{1FB924AD-1C13-C247-A903-E33A59E35643}"/>
     <hyperlink ref="G13" r:id="rId13" xr:uid="{4794E8FF-98EB-7241-A58C-377C42ED4D58}"/>
+    <hyperlink ref="G9" r:id="rId14" xr:uid="{9719F490-0B79-DE42-B18C-A1B2E8A2FF8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
BR Nome ExameGal -LOINC
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Alergias/Modelo lógicoAlergiaIPS.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Alergias/Modelo lógicoAlergiaIPS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Alergias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787033EF-3C74-5B43-96D6-037C8C10DDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D219F9-2788-A74E-940C-A68A12E3AC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="3360" windowWidth="30240" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALergias" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="132">
   <si>
     <t>RNDS</t>
   </si>
@@ -429,6 +429,12 @@
   </si>
   <si>
     <t>http://www.saude.gov.br/fhir/r4/ValueSet/BRAlergenos-1.0   inclui conceitos de http://www.saude.gov.br/fhir/r4/CodeSystem/BRAlergenosCBARA ; http://www.saude.gov.br/fhir/r4/CodeSystem/BRImunobiologico;  http://www.saude.gov.br/fhir/r4/CodeSystem/BRMedicamento</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/uv/ips/ValueSet/allergy-intolerance-snomed-ct-ips-free-set</t>
+  </si>
+  <si>
+    <t>Binding adicional para o elemento  code</t>
   </si>
 </sst>
 </file>
@@ -659,7 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -695,10 +701,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1030,8 +1034,8 @@
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1060,8 +1064,8 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1168,7 +1172,7 @@
       <c r="M4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="N4" s="30" t="s">
+      <c r="N4" s="29" t="s">
         <v>120</v>
       </c>
       <c r="O4" s="7" t="s">
@@ -1212,7 +1216,7 @@
       <c r="M5" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="N5" s="30" t="s">
+      <c r="N5" s="29" t="s">
         <v>120</v>
       </c>
       <c r="O5" s="7" t="s">
@@ -1258,13 +1262,13 @@
       <c r="M6" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="N6" s="30" t="s">
+      <c r="N6" s="29" t="s">
         <v>120</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="P6" s="29" t="s">
+      <c r="P6" s="7" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1307,10 +1311,10 @@
       <c r="N7" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="29" t="s">
+      <c r="O7" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="P7" s="29" t="s">
+      <c r="P7" s="7" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1376,10 +1380,10 @@
       <c r="G9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H9" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="31" t="s">
         <v>129</v>
       </c>
       <c r="J9" s="16" t="s">
@@ -1439,7 +1443,7 @@
       <c r="F11" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="31"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="15" t="s">
@@ -1493,8 +1497,8 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
       <c r="J13" s="18"/>
       <c r="K13" s="16"/>
       <c r="L13" s="8"/>
@@ -1538,6 +1542,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G17" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>12</v>
@@ -1546,7 +1558,7 @@
       <c r="I18" s="26"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G19" t="s">
+      <c r="G19" s="24" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1569,9 +1581,10 @@
     <hyperlink ref="A9" r:id="rId11" xr:uid="{7FDF6F92-C7FD-B14F-8A30-255692D0FC2D}"/>
     <hyperlink ref="G9" r:id="rId12" xr:uid="{9719F490-0B79-DE42-B18C-A1B2E8A2FF8E}"/>
     <hyperlink ref="G10" r:id="rId13" display="http://hl7.org/fhir/uv/ips/ValueSet/allergy-intolerance-uv-ips" xr:uid="{7FDA013E-6A26-1A44-8B42-C9A2AA79AC6A}"/>
+    <hyperlink ref="G17" r:id="rId14" xr:uid="{669767C5-F0F8-1D49-B656-AD897C6E149E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>